<commit_message>
Updates to acquisition log.csv and parts list
</commit_message>
<xml_diff>
--- a/Parts_Actual_Costs.xlsx
+++ b/Parts_Actual_Costs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15772" windowHeight="10555" xr2:uid="{E98E70A6-6B19-4DB8-B9CD-10E6A2AE4743}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15772" windowHeight="10012" xr2:uid="{E98E70A6-6B19-4DB8-B9CD-10E6A2AE4743}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Item</t>
   </si>
@@ -89,9 +89,6 @@
     <t>USB Micro-B Power Breakout</t>
   </si>
   <si>
-    <t>ebay</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -102,6 +99,33 @@
   </si>
   <si>
     <t>uBlox GPS</t>
+  </si>
+  <si>
+    <t>Unique Photo</t>
+  </si>
+  <si>
+    <t>GND2353</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>DEV-13743</t>
+  </si>
+  <si>
+    <t>Nylon tactical belt</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Waterproof airtight survival case</t>
+  </si>
+  <si>
+    <t>5v 5600 mAh USB battery</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -125,12 +149,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,9 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5477E64E-2283-47DE-BE70-0217F6914895}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -478,7 +516,7 @@
     <col min="7" max="7" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -526,7 +564,7 @@
         <v>0.77159999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -550,7 +588,7 @@
         <v>5.7200000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -570,11 +608,14 @@
         <v>4</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G7" si="0">(D4+E4)/F4</f>
+        <f t="shared" ref="G4:G16" si="0">(D4+E4)/F4</f>
         <v>6.0875000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -598,70 +639,223 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>15.99</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>3.198</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>1.46</v>
+        <v>33.75</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1.5419999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3">
+        <v>111.5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>4.46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>174.75</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>6.99</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>312.5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>13.57</v>
+      </c>
+      <c r="F10" s="2">
+        <v>25</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>13.0428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>7.99</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>7.99</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>3.28</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <f>SUM(G2:G16)</f>
-        <v>11.7393</v>
+        <v>57.584100000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to costs and script cleanup
</commit_message>
<xml_diff>
--- a/Parts_Actual_Costs.xlsx
+++ b/Parts_Actual_Costs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Heat-shrink tubing, 50mm</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -764,7 +767,7 @@
         <v>30</v>
       </c>
       <c r="D11">
-        <v>7.99</v>
+        <v>5.99</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -774,7 +777,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>7.99</v>
+        <v>5.99</v>
       </c>
       <c r="H11" t="s">
         <v>33</v>
@@ -788,7 +791,7 @@
         <v>30</v>
       </c>
       <c r="D12">
-        <v>3.28</v>
+        <v>4.96</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -798,7 +801,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>3.28</v>
+        <v>4.96</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -823,12 +826,24 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>5.43</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
       <c r="F14">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -850,12 +865,17 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
         <f>SUM(G2:G16)</f>
-        <v>57.584100000000007</v>
+        <v>57.445100000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>